<commit_message>
Update 1.2: Edits for input and output; change of output template excel file
</commit_message>
<xml_diff>
--- a/pkg/excels/templates/Invoice Output Report.xlsx
+++ b/pkg/excels/templates/Invoice Output Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mamad\OneDrive\Desktop\ТГЭМ\backend-v2\pkg\excels\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3759EF-9A43-45ED-B57F-063AF5840DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE553F7-1783-4775-AECA-CBCFCC01FEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Код</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>Получатель</t>
-  </si>
-  <si>
-    <t>Объект</t>
   </si>
   <si>
     <t>Бригада</t>
@@ -384,21 +381,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,9 +425,6 @@
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 1.3: Added Object Spenditure Report and other
</commit_message>
<xml_diff>
--- a/pkg/excels/templates/Invoice Output Report.xlsx
+++ b/pkg/excels/templates/Invoice Output Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mamad\OneDrive\Desktop\ТГЭМ\backend-v2\pkg\excels\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE553F7-1783-4775-AECA-CBCFCC01FEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C2856F-A460-428A-B7DA-394705DF729A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Код</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Примичание</t>
+  </si>
+  <si>
+    <t>Бригадир</t>
   </si>
 </sst>
 </file>
@@ -381,21 +384,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -409,21 +414,24 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>